<commit_message>
Updated files to include SAM and test analysis
</commit_message>
<xml_diff>
--- a/DataAnalysis/ARPY5Data.xlsx
+++ b/DataAnalysis/ARPY5Data.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edriklee/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC35DCD-F88E-C749-9385-06F614CB924A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BD98CE-D145-3049-B7D9-7237327B32D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{DC25EDB2-1C08-C74E-9123-28352745B869}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{DC25EDB2-1C08-C74E-9123-28352745B869}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="8" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="11" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="44">
   <si>
     <t>Text</t>
   </si>
@@ -149,6 +154,24 @@
   </si>
   <si>
     <t>llm</t>
+  </si>
+  <si>
+    <t>Text1</t>
+  </si>
+  <si>
+    <t>Text2</t>
+  </si>
+  <si>
+    <t>Text3</t>
+  </si>
+  <si>
+    <t>LLM1</t>
+  </si>
+  <si>
+    <t>LLM2</t>
+  </si>
+  <si>
+    <t>LLM3</t>
   </si>
 </sst>
 </file>
@@ -335,6 +358,922 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="DeepData"/>
+      <sheetName val="Window Segmentation"/>
+      <sheetName val="Segmentation 2 "/>
+      <sheetName val="7Data"/>
+      <sheetName val="DeepCleanA"/>
+      <sheetName val="DeepCleanB"/>
+      <sheetName val="Deep7DA"/>
+      <sheetName val="DeepV7DA"/>
+      <sheetName val="DeepDA"/>
+      <sheetName val="TestDA"/>
+      <sheetName val="SAMDA"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="5">
+          <cell r="AB5">
+            <v>4</v>
+          </cell>
+          <cell r="AC5">
+            <v>6</v>
+          </cell>
+          <cell r="AD5">
+            <v>5</v>
+          </cell>
+          <cell r="AE5">
+            <v>1</v>
+          </cell>
+          <cell r="AG5">
+            <v>6</v>
+          </cell>
+          <cell r="AH5">
+            <v>5</v>
+          </cell>
+          <cell r="AI5">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="AB6">
+            <v>2</v>
+          </cell>
+          <cell r="AC6">
+            <v>8</v>
+          </cell>
+          <cell r="AD6">
+            <v>5</v>
+          </cell>
+          <cell r="AE6">
+            <v>9</v>
+          </cell>
+          <cell r="AG6">
+            <v>6</v>
+          </cell>
+          <cell r="AH6">
+            <v>9</v>
+          </cell>
+          <cell r="AI6">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AB7">
+            <v>2</v>
+          </cell>
+          <cell r="AC7">
+            <v>5</v>
+          </cell>
+          <cell r="AD7">
+            <v>3</v>
+          </cell>
+          <cell r="AE7">
+            <v>3</v>
+          </cell>
+          <cell r="AG7">
+            <v>5</v>
+          </cell>
+          <cell r="AH7">
+            <v>3</v>
+          </cell>
+          <cell r="AI7">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="AB8">
+            <v>3</v>
+          </cell>
+          <cell r="AC8">
+            <v>4</v>
+          </cell>
+          <cell r="AD8">
+            <v>2</v>
+          </cell>
+          <cell r="AE8">
+            <v>1</v>
+          </cell>
+          <cell r="AG8">
+            <v>4</v>
+          </cell>
+          <cell r="AH8">
+            <v>1</v>
+          </cell>
+          <cell r="AI8">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="AB9">
+            <v>4</v>
+          </cell>
+          <cell r="AC9">
+            <v>7</v>
+          </cell>
+          <cell r="AD9">
+            <v>6</v>
+          </cell>
+          <cell r="AE9">
+            <v>4</v>
+          </cell>
+          <cell r="AG9">
+            <v>8</v>
+          </cell>
+          <cell r="AH9">
+            <v>7</v>
+          </cell>
+          <cell r="AI9">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="AB10">
+            <v>6</v>
+          </cell>
+          <cell r="AC10">
+            <v>5</v>
+          </cell>
+          <cell r="AD10">
+            <v>3</v>
+          </cell>
+          <cell r="AE10">
+            <v>3</v>
+          </cell>
+          <cell r="AG10">
+            <v>6</v>
+          </cell>
+          <cell r="AH10">
+            <v>5</v>
+          </cell>
+          <cell r="AI10">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="AB11">
+            <v>1</v>
+          </cell>
+          <cell r="AC11">
+            <v>5</v>
+          </cell>
+          <cell r="AD11">
+            <v>6</v>
+          </cell>
+          <cell r="AE11">
+            <v>6</v>
+          </cell>
+          <cell r="AG11">
+            <v>6</v>
+          </cell>
+          <cell r="AH11">
+            <v>6</v>
+          </cell>
+          <cell r="AI11">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="AB12">
+            <v>2</v>
+          </cell>
+          <cell r="AC12">
+            <v>7</v>
+          </cell>
+          <cell r="AD12">
+            <v>6</v>
+          </cell>
+          <cell r="AE12">
+            <v>7</v>
+          </cell>
+          <cell r="AG12">
+            <v>6</v>
+          </cell>
+          <cell r="AH12">
+            <v>5</v>
+          </cell>
+          <cell r="AI12">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="AB13">
+            <v>4</v>
+          </cell>
+          <cell r="AC13">
+            <v>6</v>
+          </cell>
+          <cell r="AD13">
+            <v>7</v>
+          </cell>
+          <cell r="AE13">
+            <v>4</v>
+          </cell>
+          <cell r="AG13">
+            <v>8</v>
+          </cell>
+          <cell r="AH13">
+            <v>7</v>
+          </cell>
+          <cell r="AI13">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="AB14">
+            <v>1</v>
+          </cell>
+          <cell r="AC14">
+            <v>7</v>
+          </cell>
+          <cell r="AD14">
+            <v>8</v>
+          </cell>
+          <cell r="AE14">
+            <v>6</v>
+          </cell>
+          <cell r="AG14">
+            <v>9</v>
+          </cell>
+          <cell r="AH14">
+            <v>8</v>
+          </cell>
+          <cell r="AI14">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="AB15">
+            <v>4</v>
+          </cell>
+          <cell r="AC15">
+            <v>8</v>
+          </cell>
+          <cell r="AD15">
+            <v>7</v>
+          </cell>
+          <cell r="AE15">
+            <v>7</v>
+          </cell>
+          <cell r="AG15">
+            <v>9</v>
+          </cell>
+          <cell r="AH15">
+            <v>9</v>
+          </cell>
+          <cell r="AI15">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AB16">
+            <v>0</v>
+          </cell>
+          <cell r="AC16">
+            <v>5</v>
+          </cell>
+          <cell r="AD16">
+            <v>6</v>
+          </cell>
+          <cell r="AE16">
+            <v>5</v>
+          </cell>
+          <cell r="AG16">
+            <v>5</v>
+          </cell>
+          <cell r="AH16">
+            <v>5</v>
+          </cell>
+          <cell r="AI16">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="AB17">
+            <v>3</v>
+          </cell>
+          <cell r="AC17">
+            <v>5</v>
+          </cell>
+          <cell r="AD17">
+            <v>9</v>
+          </cell>
+          <cell r="AE17">
+            <v>3</v>
+          </cell>
+          <cell r="AG17">
+            <v>9</v>
+          </cell>
+          <cell r="AH17">
+            <v>7</v>
+          </cell>
+          <cell r="AI17">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="AB18">
+            <v>4</v>
+          </cell>
+          <cell r="AC18">
+            <v>7</v>
+          </cell>
+          <cell r="AD18">
+            <v>6</v>
+          </cell>
+          <cell r="AE18">
+            <v>8</v>
+          </cell>
+          <cell r="AG18">
+            <v>5</v>
+          </cell>
+          <cell r="AH18">
+            <v>3</v>
+          </cell>
+          <cell r="AI18">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="AB19">
+            <v>3</v>
+          </cell>
+          <cell r="AC19">
+            <v>7</v>
+          </cell>
+          <cell r="AD19">
+            <v>6</v>
+          </cell>
+          <cell r="AE19">
+            <v>7</v>
+          </cell>
+          <cell r="AG19">
+            <v>7</v>
+          </cell>
+          <cell r="AH19">
+            <v>5</v>
+          </cell>
+          <cell r="AI19">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="AB20">
+            <v>3</v>
+          </cell>
+          <cell r="AC20">
+            <v>8</v>
+          </cell>
+          <cell r="AD20">
+            <v>7</v>
+          </cell>
+          <cell r="AE20">
+            <v>6</v>
+          </cell>
+          <cell r="AG20">
+            <v>7</v>
+          </cell>
+          <cell r="AH20">
+            <v>7</v>
+          </cell>
+          <cell r="AI20">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="AB21">
+            <v>4</v>
+          </cell>
+          <cell r="AC21">
+            <v>5</v>
+          </cell>
+          <cell r="AD21">
+            <v>5</v>
+          </cell>
+          <cell r="AE21">
+            <v>5</v>
+          </cell>
+          <cell r="AG21">
+            <v>5</v>
+          </cell>
+          <cell r="AH21">
+            <v>6</v>
+          </cell>
+          <cell r="AI21">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="AB22">
+            <v>5</v>
+          </cell>
+          <cell r="AC22">
+            <v>5</v>
+          </cell>
+          <cell r="AD22">
+            <v>4</v>
+          </cell>
+          <cell r="AE22">
+            <v>4</v>
+          </cell>
+          <cell r="AG22">
+            <v>6</v>
+          </cell>
+          <cell r="AH22">
+            <v>3</v>
+          </cell>
+          <cell r="AI22">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="AB23">
+            <v>3</v>
+          </cell>
+          <cell r="AC23">
+            <v>6</v>
+          </cell>
+          <cell r="AD23">
+            <v>5</v>
+          </cell>
+          <cell r="AE23">
+            <v>3</v>
+          </cell>
+          <cell r="AG23">
+            <v>8</v>
+          </cell>
+          <cell r="AH23">
+            <v>8</v>
+          </cell>
+          <cell r="AI23">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="AB24">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="AB25">
+            <v>4</v>
+          </cell>
+          <cell r="AC25">
+            <v>9</v>
+          </cell>
+          <cell r="AD25">
+            <v>9</v>
+          </cell>
+          <cell r="AE25">
+            <v>9</v>
+          </cell>
+          <cell r="AG25">
+            <v>9</v>
+          </cell>
+          <cell r="AH25">
+            <v>9</v>
+          </cell>
+          <cell r="AI25">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="AA89">
+            <v>4</v>
+          </cell>
+          <cell r="AB89">
+            <v>9</v>
+          </cell>
+          <cell r="AC89">
+            <v>9</v>
+          </cell>
+          <cell r="AD89">
+            <v>9</v>
+          </cell>
+          <cell r="AF89">
+            <v>9</v>
+          </cell>
+          <cell r="AG89">
+            <v>9</v>
+          </cell>
+          <cell r="AH89">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="AA90">
+            <v>4</v>
+          </cell>
+          <cell r="AB90">
+            <v>5.5</v>
+          </cell>
+          <cell r="AC90">
+            <v>4.5</v>
+          </cell>
+          <cell r="AD90">
+            <v>4</v>
+          </cell>
+          <cell r="AF90">
+            <v>7</v>
+          </cell>
+          <cell r="AG90">
+            <v>5</v>
+          </cell>
+          <cell r="AH90">
+            <v>6.5</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="AA91">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="AA92">
+            <v>4</v>
+          </cell>
+          <cell r="AB92">
+            <v>9</v>
+          </cell>
+          <cell r="AC92">
+            <v>6</v>
+          </cell>
+          <cell r="AD92">
+            <v>7</v>
+          </cell>
+          <cell r="AF92">
+            <v>9</v>
+          </cell>
+          <cell r="AG92">
+            <v>6</v>
+          </cell>
+          <cell r="AH92">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="AA93">
+            <v>3</v>
+          </cell>
+          <cell r="AB93">
+            <v>9</v>
+          </cell>
+          <cell r="AC93">
+            <v>8</v>
+          </cell>
+          <cell r="AD93">
+            <v>8</v>
+          </cell>
+          <cell r="AF93">
+            <v>9</v>
+          </cell>
+          <cell r="AG93">
+            <v>8</v>
+          </cell>
+          <cell r="AH93">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="AA94">
+            <v>5</v>
+          </cell>
+          <cell r="AB94">
+            <v>0</v>
+          </cell>
+          <cell r="AC94">
+            <v>6</v>
+          </cell>
+          <cell r="AD94">
+            <v>8</v>
+          </cell>
+          <cell r="AF94">
+            <v>8</v>
+          </cell>
+          <cell r="AG94">
+            <v>8</v>
+          </cell>
+          <cell r="AH94">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="AA95">
+            <v>5</v>
+          </cell>
+          <cell r="AB95">
+            <v>9</v>
+          </cell>
+          <cell r="AC95">
+            <v>6</v>
+          </cell>
+          <cell r="AD95">
+            <v>7</v>
+          </cell>
+          <cell r="AF95">
+            <v>8</v>
+          </cell>
+          <cell r="AG95">
+            <v>6</v>
+          </cell>
+          <cell r="AH95">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="AA96">
+            <v>3</v>
+          </cell>
+          <cell r="AB96">
+            <v>8</v>
+          </cell>
+          <cell r="AC96">
+            <v>6</v>
+          </cell>
+          <cell r="AD96">
+            <v>5</v>
+          </cell>
+          <cell r="AF96">
+            <v>5</v>
+          </cell>
+          <cell r="AG96">
+            <v>4</v>
+          </cell>
+          <cell r="AH96">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="AA97">
+            <v>4</v>
+          </cell>
+          <cell r="AB97">
+            <v>9</v>
+          </cell>
+          <cell r="AC97">
+            <v>8</v>
+          </cell>
+          <cell r="AD97">
+            <v>9</v>
+          </cell>
+          <cell r="AF97">
+            <v>5</v>
+          </cell>
+          <cell r="AG97">
+            <v>5</v>
+          </cell>
+          <cell r="AH97">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="AA98">
+            <v>3</v>
+          </cell>
+          <cell r="AB98">
+            <v>5</v>
+          </cell>
+          <cell r="AC98">
+            <v>6</v>
+          </cell>
+          <cell r="AD98">
+            <v>3</v>
+          </cell>
+          <cell r="AF98">
+            <v>6</v>
+          </cell>
+          <cell r="AG98">
+            <v>5</v>
+          </cell>
+          <cell r="AH98">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="AA99">
+            <v>5</v>
+          </cell>
+          <cell r="AB99">
+            <v>7</v>
+          </cell>
+          <cell r="AC99">
+            <v>8</v>
+          </cell>
+          <cell r="AD99">
+            <v>6</v>
+          </cell>
+          <cell r="AF99">
+            <v>7</v>
+          </cell>
+          <cell r="AG99">
+            <v>8</v>
+          </cell>
+          <cell r="AH99">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="AA100">
+            <v>3</v>
+          </cell>
+          <cell r="AB100">
+            <v>7</v>
+          </cell>
+          <cell r="AC100">
+            <v>5</v>
+          </cell>
+          <cell r="AD100">
+            <v>8</v>
+          </cell>
+          <cell r="AF100">
+            <v>9</v>
+          </cell>
+          <cell r="AG100">
+            <v>7</v>
+          </cell>
+          <cell r="AH100">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="AA101">
+            <v>4</v>
+          </cell>
+          <cell r="AB101">
+            <v>5</v>
+          </cell>
+          <cell r="AC101">
+            <v>2</v>
+          </cell>
+          <cell r="AD101">
+            <v>5</v>
+          </cell>
+          <cell r="AF101">
+            <v>8</v>
+          </cell>
+          <cell r="AG101">
+            <v>7</v>
+          </cell>
+          <cell r="AH101">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="AA102">
+            <v>5</v>
+          </cell>
+          <cell r="AB102">
+            <v>9</v>
+          </cell>
+          <cell r="AC102">
+            <v>5</v>
+          </cell>
+          <cell r="AD102">
+            <v>5</v>
+          </cell>
+          <cell r="AF102">
+            <v>9</v>
+          </cell>
+          <cell r="AG102">
+            <v>5</v>
+          </cell>
+          <cell r="AH102">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="AA103">
+            <v>2</v>
+          </cell>
+          <cell r="AB103">
+            <v>7</v>
+          </cell>
+          <cell r="AC103">
+            <v>7</v>
+          </cell>
+          <cell r="AD103">
+            <v>7</v>
+          </cell>
+          <cell r="AF103">
+            <v>7</v>
+          </cell>
+          <cell r="AG103">
+            <v>6</v>
+          </cell>
+          <cell r="AH103">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="AA104">
+            <v>5</v>
+          </cell>
+          <cell r="AB104">
+            <v>8</v>
+          </cell>
+          <cell r="AC104">
+            <v>7</v>
+          </cell>
+          <cell r="AD104">
+            <v>9</v>
+          </cell>
+          <cell r="AF104">
+            <v>6</v>
+          </cell>
+          <cell r="AG104">
+            <v>7</v>
+          </cell>
+          <cell r="AH104">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="AA105">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="AA106">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="AA107">
+            <v>4</v>
+          </cell>
+          <cell r="AB107">
+            <v>7</v>
+          </cell>
+          <cell r="AC107">
+            <v>6</v>
+          </cell>
+          <cell r="AD107">
+            <v>5</v>
+          </cell>
+          <cell r="AF107">
+            <v>5</v>
+          </cell>
+          <cell r="AG107">
+            <v>6</v>
+          </cell>
+          <cell r="AH107">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="AA108">
+            <v>2</v>
+          </cell>
+          <cell r="AB108">
+            <v>6</v>
+          </cell>
+          <cell r="AC108">
+            <v>7</v>
+          </cell>
+          <cell r="AD108">
+            <v>9</v>
+          </cell>
+          <cell r="AF108">
+            <v>8</v>
+          </cell>
+          <cell r="AG108">
+            <v>7</v>
+          </cell>
+          <cell r="AH108">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="AF109">
+            <v>5</v>
+          </cell>
+          <cell r="AG109">
+            <v>3</v>
+          </cell>
+          <cell r="AH109">
+            <v>4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4569,7 +5508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943F0DA2-9471-9944-A325-7EA928C34C9D}">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -6794,4 +7733,1244 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4CBEBC-EEFE-9842-9461-EED79D00BB8C}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <f>[1]DeepData!AB5</f>
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f>[1]DeepData!AA89</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <f>[1]DeepData!AB6</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>[1]DeepData!AA90</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <f>[1]DeepData!AB7</f>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>[1]DeepData!AA91</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <f>[1]DeepData!AB8</f>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f>[1]DeepData!AA92</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <f>[1]DeepData!AB9</f>
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>[1]DeepData!AA93</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <f>[1]DeepData!AB10</f>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>[1]DeepData!AA94</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <f>[1]DeepData!AB11</f>
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>[1]DeepData!AA95</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <f>[1]DeepData!AB12</f>
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f>[1]DeepData!AA96</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <f>[1]DeepData!AB13</f>
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <f>[1]DeepData!AA97</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <f>[1]DeepData!AB14</f>
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f>[1]DeepData!AA98</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <f>[1]DeepData!AB15</f>
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <f>[1]DeepData!AA99</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <f>[1]DeepData!AB16</f>
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <f>[1]DeepData!AA100</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <f>[1]DeepData!AB17</f>
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f>[1]DeepData!AA101</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <f>[1]DeepData!AB18</f>
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <f>[1]DeepData!AA102</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <f>[1]DeepData!AB19</f>
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <f>[1]DeepData!AA103</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <f>[1]DeepData!AB20</f>
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <f>[1]DeepData!AA104</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <f>[1]DeepData!AB21</f>
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <f>[1]DeepData!AA105</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <f>[1]DeepData!AB22</f>
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <f>[1]DeepData!AA106</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <f>[1]DeepData!AB23</f>
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <f>[1]DeepData!AA107</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <f>[1]DeepData!AB24</f>
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <f>[1]DeepData!AA108</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <f>[1]DeepData!AB25</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5AC6CC-C85B-6E45-98A4-0A9E20EE2E5A}">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <f>[1]DeepData!AF89</f>
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <f>[1]DeepData!AG89</f>
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <f>[1]DeepData!AH89</f>
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <f>[1]DeepData!AB89</f>
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <f>[1]DeepData!AC89</f>
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <f>[1]DeepData!AD89</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <f>[1]DeepData!AF90</f>
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <f>[1]DeepData!AG90</f>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f>[1]DeepData!AH90</f>
+        <v>6.5</v>
+      </c>
+      <c r="D3">
+        <f>[1]DeepData!AB90</f>
+        <v>5.5</v>
+      </c>
+      <c r="E3">
+        <f>[1]DeepData!AC90</f>
+        <v>4.5</v>
+      </c>
+      <c r="F3">
+        <f>[1]DeepData!AD90</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <f>[1]DeepData!AF92</f>
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <f>[1]DeepData!AG92</f>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f>[1]DeepData!AH92</f>
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <f>[1]DeepData!AB92</f>
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <f>[1]DeepData!AC92</f>
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <f>[1]DeepData!AD92</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <f>[1]DeepData!AF93</f>
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <f>[1]DeepData!AG93</f>
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f>[1]DeepData!AH93</f>
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <f>[1]DeepData!AB93</f>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f>[1]DeepData!AC93</f>
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <f>[1]DeepData!AD93</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <f>[1]DeepData!AF94</f>
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>[1]DeepData!AG94</f>
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <f>[1]DeepData!AH94</f>
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <f>[1]DeepData!AB94</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>[1]DeepData!AC94</f>
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <f>[1]DeepData!AD94</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <f>[1]DeepData!AF95</f>
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f>[1]DeepData!AG95</f>
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>[1]DeepData!AH95</f>
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <f>[1]DeepData!AB95</f>
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <f>[1]DeepData!AC95</f>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f>[1]DeepData!AD95</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <f>[1]DeepData!AF96</f>
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <f>[1]DeepData!AG96</f>
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f>[1]DeepData!AH96</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f>[1]DeepData!AB96</f>
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <f>[1]DeepData!AC96</f>
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f>[1]DeepData!AD96</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <f>[1]DeepData!AF97</f>
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <f>[1]DeepData!AG97</f>
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f>[1]DeepData!AH97</f>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f>[1]DeepData!AB97</f>
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <f>[1]DeepData!AC97</f>
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <f>[1]DeepData!AD97</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <f>[1]DeepData!AF98</f>
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <f>[1]DeepData!AG98</f>
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f>[1]DeepData!AH98</f>
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <f>[1]DeepData!AB98</f>
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f>[1]DeepData!AC98</f>
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <f>[1]DeepData!AD98</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <f>[1]DeepData!AF99</f>
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <f>[1]DeepData!AG99</f>
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f>[1]DeepData!AH99</f>
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <f>[1]DeepData!AB99</f>
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <f>[1]DeepData!AC99</f>
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <f>[1]DeepData!AD99</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <f>[1]DeepData!AF100</f>
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <f>[1]DeepData!AG100</f>
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <f>[1]DeepData!AH100</f>
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f>[1]DeepData!AB100</f>
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <f>[1]DeepData!AC100</f>
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <f>[1]DeepData!AD100</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <f>[1]DeepData!AF101</f>
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <f>[1]DeepData!AG101</f>
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <f>[1]DeepData!AH101</f>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f>[1]DeepData!AB101</f>
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <f>[1]DeepData!AC101</f>
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <f>[1]DeepData!AD101</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <f>[1]DeepData!AF102</f>
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <f>[1]DeepData!AG102</f>
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f>[1]DeepData!AH102</f>
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <f>[1]DeepData!AB102</f>
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <f>[1]DeepData!AC102</f>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f>[1]DeepData!AD102</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <f>[1]DeepData!AF103</f>
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <f>[1]DeepData!AG103</f>
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <f>[1]DeepData!AH103</f>
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <f>[1]DeepData!AB103</f>
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <f>[1]DeepData!AC103</f>
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <f>[1]DeepData!AD103</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <f>[1]DeepData!AF104</f>
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <f>[1]DeepData!AG104</f>
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <f>[1]DeepData!AH104</f>
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <f>[1]DeepData!AB104</f>
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <f>[1]DeepData!AC104</f>
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <f>[1]DeepData!AD104</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <f>[1]DeepData!AF107</f>
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <f>[1]DeepData!AG107</f>
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <f>[1]DeepData!AH107</f>
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f>[1]DeepData!AB107</f>
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <f>[1]DeepData!AC107</f>
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <f>[1]DeepData!AD107</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <f>[1]DeepData!AF108</f>
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <f>[1]DeepData!AG108</f>
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <f>[1]DeepData!AH108</f>
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <f>[1]DeepData!AB108</f>
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <f>[1]DeepData!AC108</f>
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <f>[1]DeepData!AD108</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <f>[1]DeepData!AF109</f>
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <f>[1]DeepData!AG109</f>
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <f>[1]DeepData!AH109</f>
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <f>[1]DeepData!AG5</f>
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <f>[1]DeepData!AH5</f>
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <f>[1]DeepData!AI5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <f>[1]DeepData!AC5</f>
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <f>[1]DeepData!AD5</f>
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <f>[1]DeepData!AE5</f>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>[1]DeepData!AG6</f>
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <f>[1]DeepData!AH6</f>
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <f>[1]DeepData!AI6</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <f>[1]DeepData!AC6</f>
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <f>[1]DeepData!AD6</f>
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <f>[1]DeepData!AE6</f>
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <f>[1]DeepData!AG7</f>
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <f>[1]DeepData!AH7</f>
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <f>[1]DeepData!AI7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <f>[1]DeepData!AC7</f>
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <f>[1]DeepData!AD7</f>
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <f>[1]DeepData!AE7</f>
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <f>[1]DeepData!AG8</f>
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <f>[1]DeepData!AH8</f>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f>[1]DeepData!AI8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <f>[1]DeepData!AC8</f>
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <f>[1]DeepData!AD8</f>
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <f>[1]DeepData!AE8</f>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>[1]DeepData!AG9</f>
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <f>[1]DeepData!AH9</f>
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <f>[1]DeepData!AI9</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <f>[1]DeepData!AC9</f>
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <f>[1]DeepData!AD9</f>
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <f>[1]DeepData!AE9</f>
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <f>[1]DeepData!AG10</f>
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <f>[1]DeepData!AH10</f>
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <f>[1]DeepData!AI10</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <f>[1]DeepData!AC10</f>
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <f>[1]DeepData!AD10</f>
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <f>[1]DeepData!AE10</f>
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <f>[1]DeepData!AG11</f>
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <f>[1]DeepData!AH11</f>
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <f>[1]DeepData!AI11</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <f>[1]DeepData!AC11</f>
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <f>[1]DeepData!AD11</f>
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <f>[1]DeepData!AE11</f>
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <f>[1]DeepData!AG12</f>
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <f>[1]DeepData!AH12</f>
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <f>[1]DeepData!AI12</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <f>[1]DeepData!AC12</f>
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <f>[1]DeepData!AD12</f>
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <f>[1]DeepData!AE12</f>
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <f>[1]DeepData!AG13</f>
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <f>[1]DeepData!AH13</f>
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <f>[1]DeepData!AI13</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <f>[1]DeepData!AC13</f>
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <f>[1]DeepData!AD13</f>
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <f>[1]DeepData!AE13</f>
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <f>[1]DeepData!AG14</f>
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <f>[1]DeepData!AH14</f>
+        <v>8</v>
+      </c>
+      <c r="F28">
+        <f>[1]DeepData!AI14</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <f>[1]DeepData!AC14</f>
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <f>[1]DeepData!AD14</f>
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <f>[1]DeepData!AE14</f>
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <f>[1]DeepData!AG15</f>
+        <v>9</v>
+      </c>
+      <c r="E29">
+        <f>[1]DeepData!AH15</f>
+        <v>9</v>
+      </c>
+      <c r="F29">
+        <f>[1]DeepData!AI15</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <f>[1]DeepData!AC15</f>
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <f>[1]DeepData!AD15</f>
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <f>[1]DeepData!AE15</f>
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <f>[1]DeepData!AG16</f>
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <f>[1]DeepData!AH16</f>
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <f>[1]DeepData!AI16</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <f>[1]DeepData!AC16</f>
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <f>[1]DeepData!AD16</f>
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <f>[1]DeepData!AE16</f>
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <f>[1]DeepData!AG17</f>
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <f>[1]DeepData!AH17</f>
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <f>[1]DeepData!AI17</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <f>[1]DeepData!AC17</f>
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <f>[1]DeepData!AD17</f>
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <f>[1]DeepData!AE17</f>
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <f>[1]DeepData!AG18</f>
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <f>[1]DeepData!AH18</f>
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f>[1]DeepData!AI18</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <f>[1]DeepData!AC18</f>
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <f>[1]DeepData!AD18</f>
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <f>[1]DeepData!AE18</f>
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <f>[1]DeepData!AG19</f>
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <f>[1]DeepData!AH19</f>
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <f>[1]DeepData!AI19</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <f>[1]DeepData!AC19</f>
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <f>[1]DeepData!AD19</f>
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <f>[1]DeepData!AE19</f>
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <f>[1]DeepData!AG20</f>
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <f>[1]DeepData!AH20</f>
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <f>[1]DeepData!AI20</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <f>[1]DeepData!AC20</f>
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <f>[1]DeepData!AD20</f>
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <f>[1]DeepData!AE20</f>
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <f>[1]DeepData!AG21</f>
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <f>[1]DeepData!AH21</f>
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <f>[1]DeepData!AI21</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <f>[1]DeepData!AC21</f>
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <f>[1]DeepData!AD21</f>
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <f>[1]DeepData!AE21</f>
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <f>[1]DeepData!AG22</f>
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <f>[1]DeepData!AH22</f>
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <f>[1]DeepData!AI22</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <f>[1]DeepData!AC22</f>
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <f>[1]DeepData!AD22</f>
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <f>[1]DeepData!AE22</f>
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <f>[1]DeepData!AG23</f>
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <f>[1]DeepData!AH23</f>
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <f>[1]DeepData!AI23</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <f>[1]DeepData!AC23</f>
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <f>[1]DeepData!AD23</f>
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <f>[1]DeepData!AE23</f>
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <f>[1]DeepData!AG25</f>
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <f>[1]DeepData!AH25</f>
+        <v>9</v>
+      </c>
+      <c r="F38">
+        <f>[1]DeepData!AI25</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <f>[1]DeepData!AC25</f>
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <f>[1]DeepData!AD25</f>
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <f>[1]DeepData!AE25</f>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>